<commit_message>
Made changes to grid connection and sun profile
</commit_message>
<xml_diff>
--- a/data/YIELD_EE.xlsx
+++ b/data/YIELD_EE.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevineriksson/PycharmProjects/Simulation/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D7A1C5C-1AD5-0E48-AAC4-CFE76D4934D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D03672CC-C771-6140-A553-5C70E8C394BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7800" yWindow="2380" windowWidth="27240" windowHeight="17880" xr2:uid="{B2249A4F-5109-C145-A437-E2DC31518187}"/>
+    <workbookView xWindow="6960" yWindow="780" windowWidth="27240" windowHeight="19660" xr2:uid="{B2249A4F-5109-C145-A437-E2DC31518187}"/>
   </bookViews>
   <sheets>
     <sheet name="Yearly" sheetId="1" r:id="rId1"/>
@@ -441,7 +441,7 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -502,7 +502,7 @@
         <v>2800</v>
       </c>
       <c r="C5" s="3">
-        <v>817.79187192118229</v>
+        <v>1100</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -513,7 +513,7 @@
         <v>3300</v>
       </c>
       <c r="C6" s="3">
-        <v>820.13760330578509</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>